<commit_message>
Modification sur le comparatif analytique
</commit_message>
<xml_diff>
--- a/AutosurveillanceTemplates/Comparatif.xlsx
+++ b/AutosurveillanceTemplates/Comparatif.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\ndhuy\AppData\Roaming\Microsoft\AddIns\AutosurveillanceTemplates\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C722C51D-CB80-4528-A5F0-85F5289FE611}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F444B865-2AFB-4C37-BF82-A1A9DF9FC4AF}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-28920" yWindow="3135" windowWidth="29040" windowHeight="15720" activeTab="1" xr2:uid="{A7F306DE-866C-4C6A-BADD-FDD34CC5E268}"/>
   </bookViews>
@@ -443,7 +443,7 @@
       </patternFill>
     </fill>
   </fills>
-  <borders count="52">
+  <borders count="54">
     <border>
       <left/>
       <right/>
@@ -1120,6 +1120,30 @@
       </right>
       <top/>
       <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="medium">
+        <color indexed="64"/>
+      </left>
+      <right/>
+      <top style="hair">
+        <color indexed="64"/>
+      </top>
+      <bottom style="medium">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="medium">
+        <color indexed="64"/>
+      </left>
+      <right/>
+      <top/>
+      <bottom style="medium">
+        <color indexed="64"/>
+      </bottom>
       <diagonal/>
     </border>
   </borders>
@@ -1127,7 +1151,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="100">
+  <cellXfs count="101">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="0" xfId="1" applyFill="1" applyAlignment="1" applyProtection="1">
       <alignment vertical="center"/>
@@ -1384,10 +1408,6 @@
       <alignment horizontal="center" vertical="center"/>
       <protection locked="0" hidden="1"/>
     </xf>
-    <xf numFmtId="0" fontId="9" fillId="4" borderId="19" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="center" vertical="center"/>
-      <protection hidden="1"/>
-    </xf>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="47" xfId="1" applyBorder="1" applyAlignment="1" applyProtection="1">
       <alignment horizontal="center" vertical="center"/>
       <protection locked="0" hidden="1"/>
@@ -1403,10 +1423,6 @@
     <xf numFmtId="0" fontId="1" fillId="4" borderId="48" xfId="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
       <alignment horizontal="center" vertical="center"/>
       <protection locked="0" hidden="1"/>
-    </xf>
-    <xf numFmtId="164" fontId="1" fillId="0" borderId="35" xfId="1" applyNumberFormat="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="center" vertical="center"/>
-      <protection hidden="1"/>
     </xf>
     <xf numFmtId="0" fontId="7" fillId="4" borderId="36" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
       <alignment horizontal="center" vertical="center"/>
@@ -1431,71 +1447,83 @@
       <alignment horizontal="center" vertical="center" wrapText="1"/>
       <protection hidden="1"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="7" borderId="24" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="3" borderId="25" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+      <protection hidden="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="3" borderId="29" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+      <protection hidden="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="3" borderId="34" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+      <protection hidden="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="3" borderId="26" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+      <protection hidden="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="3" borderId="30" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+      <protection hidden="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="3" borderId="35" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+      <protection hidden="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="3" borderId="26" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="center" vertical="center" textRotation="90" wrapText="1"/>
+      <protection hidden="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="3" borderId="30" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="center" vertical="center" textRotation="90" wrapText="1"/>
+      <protection hidden="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="3" borderId="35" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="center" vertical="center" textRotation="90" wrapText="1"/>
+      <protection hidden="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="3" borderId="32" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+      <protection hidden="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="3" borderId="33" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="center" vertical="center" textRotation="90" wrapText="1"/>
+      <protection hidden="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="3" borderId="36" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="center" vertical="center" textRotation="90" wrapText="1"/>
+      <protection hidden="1"/>
+    </xf>
     <xf numFmtId="0" fontId="10" fillId="7" borderId="24" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="11" fillId="6" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="7" borderId="24" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
     <xf numFmtId="0" fontId="11" fillId="6" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="left" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="11" fillId="6" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="4" fillId="3" borderId="25" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-      <protection hidden="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="3" borderId="29" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-      <protection hidden="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="3" borderId="34" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-      <protection hidden="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="3" borderId="26" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-      <protection hidden="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="3" borderId="30" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-      <protection hidden="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="3" borderId="35" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-      <protection hidden="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="3" borderId="26" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="center" vertical="center" textRotation="90" wrapText="1"/>
-      <protection hidden="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="3" borderId="30" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="center" vertical="center" textRotation="90" wrapText="1"/>
-      <protection hidden="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="3" borderId="35" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="center" vertical="center" textRotation="90" wrapText="1"/>
-      <protection hidden="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="3" borderId="32" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-      <protection hidden="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="3" borderId="33" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="center" vertical="center" textRotation="90" wrapText="1"/>
-      <protection hidden="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="3" borderId="36" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="center" vertical="center" textRotation="90" wrapText="1"/>
-      <protection hidden="1"/>
-    </xf>
     <xf numFmtId="0" fontId="11" fillId="6" borderId="51" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="4" borderId="52" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="center" vertical="center"/>
+      <protection hidden="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="4" borderId="53" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="center" vertical="center"/>
+      <protection hidden="1"/>
+    </xf>
+    <xf numFmtId="164" fontId="1" fillId="0" borderId="35" xfId="1" applyNumberFormat="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="center" vertical="center"/>
+      <protection hidden="1"/>
     </xf>
   </cellXfs>
   <cellStyles count="2">
@@ -1842,8 +1870,8 @@
   <sheetPr codeName="Feuil1"/>
   <dimension ref="A1:K29"/>
   <sheetViews>
-    <sheetView topLeftCell="A16" workbookViewId="0">
-      <selection activeCell="M8" sqref="M8"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="H5" sqref="H5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="14.35" x14ac:dyDescent="0.5"/>
@@ -1866,17 +1894,17 @@
     </row>
     <row r="2" spans="1:11" s="3" customFormat="1" ht="15.7" thickBot="1" x14ac:dyDescent="0.55000000000000004">
       <c r="A2" s="1"/>
-      <c r="B2" s="78" t="s">
+      <c r="B2" s="76" t="s">
         <v>0</v>
       </c>
-      <c r="C2" s="79"/>
-      <c r="D2" s="79"/>
-      <c r="E2" s="79"/>
-      <c r="F2" s="79"/>
-      <c r="G2" s="79"/>
-      <c r="H2" s="79"/>
-      <c r="I2" s="79"/>
-      <c r="J2" s="80"/>
+      <c r="C2" s="77"/>
+      <c r="D2" s="77"/>
+      <c r="E2" s="77"/>
+      <c r="F2" s="77"/>
+      <c r="G2" s="77"/>
+      <c r="H2" s="77"/>
+      <c r="I2" s="77"/>
+      <c r="J2" s="78"/>
       <c r="K2" s="1"/>
     </row>
     <row r="3" spans="1:11" s="3" customFormat="1" ht="13" thickBot="1" x14ac:dyDescent="0.55000000000000004">
@@ -2578,30 +2606,30 @@
     </row>
     <row r="28" spans="1:11" s="3" customFormat="1" ht="12.75" customHeight="1" x14ac:dyDescent="0.5">
       <c r="A28" s="1"/>
-      <c r="B28" s="81" t="s">
+      <c r="B28" s="79" t="s">
         <v>39</v>
       </c>
-      <c r="C28" s="81"/>
-      <c r="D28" s="81"/>
-      <c r="E28" s="81"/>
-      <c r="F28" s="81"/>
-      <c r="G28" s="81"/>
-      <c r="H28" s="81"/>
-      <c r="I28" s="81"/>
-      <c r="J28" s="81"/>
+      <c r="C28" s="79"/>
+      <c r="D28" s="79"/>
+      <c r="E28" s="79"/>
+      <c r="F28" s="79"/>
+      <c r="G28" s="79"/>
+      <c r="H28" s="79"/>
+      <c r="I28" s="79"/>
+      <c r="J28" s="79"/>
       <c r="K28" s="1"/>
     </row>
     <row r="29" spans="1:11" s="3" customFormat="1" ht="14.35" customHeight="1" x14ac:dyDescent="0.5">
       <c r="A29" s="1"/>
-      <c r="B29" s="81"/>
-      <c r="C29" s="81"/>
-      <c r="D29" s="81"/>
-      <c r="E29" s="81"/>
-      <c r="F29" s="81"/>
-      <c r="G29" s="81"/>
-      <c r="H29" s="81"/>
-      <c r="I29" s="81"/>
-      <c r="J29" s="81"/>
+      <c r="B29" s="79"/>
+      <c r="C29" s="79"/>
+      <c r="D29" s="79"/>
+      <c r="E29" s="79"/>
+      <c r="F29" s="79"/>
+      <c r="G29" s="79"/>
+      <c r="H29" s="79"/>
+      <c r="I29" s="79"/>
+      <c r="J29" s="79"/>
       <c r="K29" s="1"/>
     </row>
   </sheetData>
@@ -2619,51 +2647,51 @@
   <sheetPr codeName="Feuil2"/>
   <dimension ref="A1:L37"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A3" sqref="A3:B3"/>
+    <sheetView tabSelected="1" topLeftCell="A4" workbookViewId="0">
+      <selection activeCell="H32" sqref="A7:H32"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="14.35" x14ac:dyDescent="0.5"/>
   <sheetData>
     <row r="1" spans="1:12" x14ac:dyDescent="0.5">
-      <c r="A1" s="75"/>
-      <c r="B1" s="75"/>
-      <c r="C1" s="76"/>
-      <c r="D1" s="75"/>
-      <c r="E1" s="75"/>
-      <c r="F1" s="75"/>
-      <c r="G1" s="75"/>
-      <c r="H1" s="75"/>
-      <c r="I1" s="75"/>
-      <c r="J1" s="77"/>
+      <c r="A1" s="73"/>
+      <c r="B1" s="73"/>
+      <c r="C1" s="74"/>
+      <c r="D1" s="73"/>
+      <c r="E1" s="73"/>
+      <c r="F1" s="73"/>
+      <c r="G1" s="73"/>
+      <c r="H1" s="73"/>
+      <c r="I1" s="73"/>
+      <c r="J1" s="75"/>
     </row>
     <row r="2" spans="1:12" x14ac:dyDescent="0.5">
-      <c r="A2" s="83" t="s">
+      <c r="A2" s="94" t="s">
         <v>54</v>
       </c>
-      <c r="B2" s="99"/>
-      <c r="C2" s="82"/>
-      <c r="D2" s="82"/>
-      <c r="E2" s="83" t="s">
+      <c r="B2" s="97"/>
+      <c r="C2" s="93"/>
+      <c r="D2" s="93"/>
+      <c r="E2" s="94" t="s">
         <v>40</v>
       </c>
-      <c r="F2" s="83"/>
-      <c r="G2" s="84"/>
-      <c r="H2" s="84"/>
+      <c r="F2" s="94"/>
+      <c r="G2" s="80"/>
+      <c r="H2" s="80"/>
       <c r="I2" s="39"/>
       <c r="J2" s="40"/>
     </row>
     <row r="3" spans="1:12" ht="27.35" customHeight="1" x14ac:dyDescent="0.5">
-      <c r="A3" s="85" t="s">
+      <c r="A3" s="95" t="s">
         <v>41</v>
       </c>
-      <c r="B3" s="85"/>
-      <c r="C3" s="82"/>
-      <c r="D3" s="82"/>
-      <c r="E3" s="86" t="s">
+      <c r="B3" s="95"/>
+      <c r="C3" s="93"/>
+      <c r="D3" s="93"/>
+      <c r="E3" s="96" t="s">
         <v>42</v>
       </c>
-      <c r="F3" s="86"/>
+      <c r="F3" s="96"/>
       <c r="G3" s="39"/>
       <c r="H3" s="39"/>
       <c r="I3" s="39"/>
@@ -2678,8 +2706,8 @@
       <c r="F4" s="42" t="s">
         <v>43</v>
       </c>
-      <c r="G4" s="84"/>
-      <c r="H4" s="84"/>
+      <c r="G4" s="80"/>
+      <c r="H4" s="80"/>
       <c r="I4" s="39"/>
       <c r="J4" s="40"/>
     </row>
@@ -2692,8 +2720,8 @@
       <c r="F5" s="42" t="s">
         <v>44</v>
       </c>
-      <c r="G5" s="84"/>
-      <c r="H5" s="84"/>
+      <c r="G5" s="80"/>
+      <c r="H5" s="80"/>
       <c r="I5" s="39"/>
       <c r="J5" s="40"/>
     </row>
@@ -2710,22 +2738,22 @@
       <c r="J6" s="40"/>
     </row>
     <row r="7" spans="1:12" x14ac:dyDescent="0.5">
-      <c r="A7" s="87" t="s">
+      <c r="A7" s="81" t="s">
         <v>2</v>
       </c>
-      <c r="B7" s="90" t="s">
+      <c r="B7" s="84" t="s">
         <v>45</v>
       </c>
-      <c r="C7" s="90" t="s">
+      <c r="C7" s="84" t="s">
         <v>46</v>
       </c>
-      <c r="D7" s="93" t="s">
+      <c r="D7" s="87" t="s">
         <v>47</v>
       </c>
-      <c r="E7" s="90" t="s">
+      <c r="E7" s="84" t="s">
         <v>48</v>
       </c>
-      <c r="F7" s="93" t="s">
+      <c r="F7" s="87" t="s">
         <v>47</v>
       </c>
       <c r="G7" s="43" t="s">
@@ -2738,12 +2766,12 @@
       <c r="J7" s="40"/>
     </row>
     <row r="8" spans="1:12" x14ac:dyDescent="0.5">
-      <c r="A8" s="88"/>
-      <c r="B8" s="91"/>
-      <c r="C8" s="91"/>
-      <c r="D8" s="94"/>
-      <c r="E8" s="91"/>
-      <c r="F8" s="94"/>
+      <c r="A8" s="82"/>
+      <c r="B8" s="85"/>
+      <c r="C8" s="85"/>
+      <c r="D8" s="88"/>
+      <c r="E8" s="85"/>
+      <c r="F8" s="88"/>
       <c r="G8" s="45">
         <f>COUNT(G11:G32)</f>
         <v>0</v>
@@ -2764,30 +2792,30 @@
       </c>
     </row>
     <row r="9" spans="1:12" x14ac:dyDescent="0.5">
-      <c r="A9" s="88"/>
-      <c r="B9" s="91"/>
-      <c r="C9" s="91"/>
-      <c r="D9" s="94"/>
-      <c r="E9" s="91"/>
-      <c r="F9" s="94"/>
-      <c r="G9" s="96" t="s">
+      <c r="A9" s="82"/>
+      <c r="B9" s="85"/>
+      <c r="C9" s="85"/>
+      <c r="D9" s="88"/>
+      <c r="E9" s="85"/>
+      <c r="F9" s="88"/>
+      <c r="G9" s="90" t="s">
         <v>51</v>
       </c>
-      <c r="H9" s="97" t="s">
+      <c r="H9" s="91" t="s">
         <v>52</v>
       </c>
       <c r="I9" s="39"/>
       <c r="J9" s="40"/>
     </row>
     <row r="10" spans="1:12" ht="43" customHeight="1" thickBot="1" x14ac:dyDescent="0.55000000000000004">
-      <c r="A10" s="89"/>
-      <c r="B10" s="92"/>
-      <c r="C10" s="92"/>
-      <c r="D10" s="95"/>
-      <c r="E10" s="92"/>
-      <c r="F10" s="95"/>
-      <c r="G10" s="92"/>
-      <c r="H10" s="98"/>
+      <c r="A10" s="83"/>
+      <c r="B10" s="86"/>
+      <c r="C10" s="86"/>
+      <c r="D10" s="89"/>
+      <c r="E10" s="86"/>
+      <c r="F10" s="89"/>
+      <c r="G10" s="86"/>
+      <c r="H10" s="92"/>
       <c r="I10" s="39"/>
       <c r="J10" s="40"/>
     </row>
@@ -2804,8 +2832,8 @@
       <c r="E11" s="52"/>
       <c r="F11" s="53"/>
       <c r="G11" s="54" t="str">
-        <f xml:space="preserve"> IF(E11&gt;0,(C11-E11)/E11,"-")</f>
-        <v>-</v>
+        <f>IF(OR(E11="",C11=""),"",IF(ISERROR(VLOOKUP(A11,'SeuilsComparaison-EMT'!$C$5:$J$25,4,FALSE)),"-",IF(OR(IF(ISTEXT(E11)=TRUE,SUBSTITUTE(E11,"&lt;","",1)*1,E11)&gt;VLOOKUP(A11,'SeuilsComparaison-EMT'!$C$5:$J$25,4,FALSE),IF(ISTEXT(C11)=TRUE,SUBSTITUTE(C11,"&lt;","",1)*1,C11)&gt;VLOOKUP(A11,'SeuilsComparaison-EMT'!$C$5:$J$25,4,FALSE)=TRUE),(IF(ISTEXT(C11)=TRUE,SUBSTITUTE(C11,"&lt;","",1)*1,C11)-((IF(ISTEXT(C11)=TRUE,SUBSTITUTE(C11,"&lt;","",1)*1,C11)+IF(ISTEXT(E11)=TRUE,SUBSTITUTE(E11,"&lt;","",1)*1,E11))/2))/((IF(ISTEXT(C11)=TRUE,SUBSTITUTE(C11,"&lt;","",1)*1,C11)+IF(ISTEXT(E11)=TRUE,SUBSTITUTE(E11,"&lt;","",1),E11))/2),"-")))</f>
+        <v/>
       </c>
       <c r="H11" s="55"/>
       <c r="I11" s="39"/>
@@ -2824,8 +2852,8 @@
       <c r="E12" s="57"/>
       <c r="F12" s="58"/>
       <c r="G12" s="54" t="str">
-        <f t="shared" ref="G12:G29" si="0" xml:space="preserve"> IF(E12&gt;0,(C12-E12)/E12,"-")</f>
-        <v>-</v>
+        <f>IF(OR(E12="",C12=""),"",IF(ISERROR(VLOOKUP(A12,'SeuilsComparaison-EMT'!$C$5:$J$25,4,FALSE)),"-",IF(OR(IF(ISTEXT(E12)=TRUE,SUBSTITUTE(E12,"&lt;","",1)*1,E12)&gt;VLOOKUP(A12,'SeuilsComparaison-EMT'!$C$5:$J$25,4,FALSE),IF(ISTEXT(C12)=TRUE,SUBSTITUTE(C12,"&lt;","",1)*1,C12)&gt;VLOOKUP(A12,'SeuilsComparaison-EMT'!$C$5:$J$25,4,FALSE)=TRUE),(IF(ISTEXT(C12)=TRUE,SUBSTITUTE(C12,"&lt;","",1)*1,C12)-((IF(ISTEXT(C12)=TRUE,SUBSTITUTE(C12,"&lt;","",1)*1,C12)+IF(ISTEXT(E12)=TRUE,SUBSTITUTE(E12,"&lt;","",1)*1,E12))/2))/((IF(ISTEXT(C12)=TRUE,SUBSTITUTE(C12,"&lt;","",1)*1,C12)+IF(ISTEXT(E12)=TRUE,SUBSTITUTE(E12,"&lt;","",1),E12))/2),"-")))</f>
+        <v/>
       </c>
       <c r="H12" s="59"/>
       <c r="I12" s="39"/>
@@ -2844,8 +2872,8 @@
       <c r="E13" s="61"/>
       <c r="F13" s="58"/>
       <c r="G13" s="54" t="str">
-        <f t="shared" si="0"/>
-        <v>-</v>
+        <f>IF(OR(E13="",C13=""),"",IF(ISERROR(VLOOKUP(A13,'SeuilsComparaison-EMT'!$C$5:$J$25,4,FALSE)),"-",IF(OR(IF(ISTEXT(E13)=TRUE,SUBSTITUTE(E13,"&lt;","",1)*1,E13)&gt;VLOOKUP(A13,'SeuilsComparaison-EMT'!$C$5:$J$25,4,FALSE),IF(ISTEXT(C13)=TRUE,SUBSTITUTE(C13,"&lt;","",1)*1,C13)&gt;VLOOKUP(A13,'SeuilsComparaison-EMT'!$C$5:$J$25,4,FALSE)=TRUE),(IF(ISTEXT(C13)=TRUE,SUBSTITUTE(C13,"&lt;","",1)*1,C13)-((IF(ISTEXT(C13)=TRUE,SUBSTITUTE(C13,"&lt;","",1)*1,C13)+IF(ISTEXT(E13)=TRUE,SUBSTITUTE(E13,"&lt;","",1)*1,E13))/2))/((IF(ISTEXT(C13)=TRUE,SUBSTITUTE(C13,"&lt;","",1)*1,C13)+IF(ISTEXT(E13)=TRUE,SUBSTITUTE(E13,"&lt;","",1),E13))/2),"-")))</f>
+        <v/>
       </c>
       <c r="H13" s="59"/>
       <c r="I13" s="39"/>
@@ -2864,8 +2892,8 @@
       <c r="E14" s="57"/>
       <c r="F14" s="58"/>
       <c r="G14" s="54" t="str">
-        <f t="shared" si="0"/>
-        <v>-</v>
+        <f>IF(OR(E14="",C14=""),"",IF(ISERROR(VLOOKUP(A14,'SeuilsComparaison-EMT'!$C$5:$J$25,4,FALSE)),"-",IF(OR(IF(ISTEXT(E14)=TRUE,SUBSTITUTE(E14,"&lt;","",1)*1,E14)&gt;VLOOKUP(A14,'SeuilsComparaison-EMT'!$C$5:$J$25,4,FALSE),IF(ISTEXT(C14)=TRUE,SUBSTITUTE(C14,"&lt;","",1)*1,C14)&gt;VLOOKUP(A14,'SeuilsComparaison-EMT'!$C$5:$J$25,4,FALSE)=TRUE),(IF(ISTEXT(C14)=TRUE,SUBSTITUTE(C14,"&lt;","",1)*1,C14)-((IF(ISTEXT(C14)=TRUE,SUBSTITUTE(C14,"&lt;","",1)*1,C14)+IF(ISTEXT(E14)=TRUE,SUBSTITUTE(E14,"&lt;","",1)*1,E14))/2))/((IF(ISTEXT(C14)=TRUE,SUBSTITUTE(C14,"&lt;","",1)*1,C14)+IF(ISTEXT(E14)=TRUE,SUBSTITUTE(E14,"&lt;","",1),E14))/2),"-")))</f>
+        <v/>
       </c>
       <c r="H14" s="59"/>
       <c r="I14" s="39"/>
@@ -2884,8 +2912,8 @@
       <c r="E15" s="57"/>
       <c r="F15" s="58"/>
       <c r="G15" s="54" t="str">
-        <f t="shared" si="0"/>
-        <v>-</v>
+        <f>IF(OR(E15="",C15=""),"",IF(ISERROR(VLOOKUP(A15,'SeuilsComparaison-EMT'!$C$5:$J$25,4,FALSE)),"-",IF(OR(IF(ISTEXT(E15)=TRUE,SUBSTITUTE(E15,"&lt;","",1)*1,E15)&gt;VLOOKUP(A15,'SeuilsComparaison-EMT'!$C$5:$J$25,4,FALSE),IF(ISTEXT(C15)=TRUE,SUBSTITUTE(C15,"&lt;","",1)*1,C15)&gt;VLOOKUP(A15,'SeuilsComparaison-EMT'!$C$5:$J$25,4,FALSE)=TRUE),(IF(ISTEXT(C15)=TRUE,SUBSTITUTE(C15,"&lt;","",1)*1,C15)-((IF(ISTEXT(C15)=TRUE,SUBSTITUTE(C15,"&lt;","",1)*1,C15)+IF(ISTEXT(E15)=TRUE,SUBSTITUTE(E15,"&lt;","",1)*1,E15))/2))/((IF(ISTEXT(C15)=TRUE,SUBSTITUTE(C15,"&lt;","",1)*1,C15)+IF(ISTEXT(E15)=TRUE,SUBSTITUTE(E15,"&lt;","",1),E15))/2),"-")))</f>
+        <v/>
       </c>
       <c r="H15" s="59"/>
       <c r="I15" s="39"/>
@@ -2904,8 +2932,8 @@
       <c r="E16" s="57"/>
       <c r="F16" s="58"/>
       <c r="G16" s="54" t="str">
-        <f t="shared" si="0"/>
-        <v>-</v>
+        <f>IF(OR(E16="",C16=""),"",IF(ISERROR(VLOOKUP(A16,'SeuilsComparaison-EMT'!$C$5:$J$25,4,FALSE)),"-",IF(OR(IF(ISTEXT(E16)=TRUE,SUBSTITUTE(E16,"&lt;","",1)*1,E16)&gt;VLOOKUP(A16,'SeuilsComparaison-EMT'!$C$5:$J$25,4,FALSE),IF(ISTEXT(C16)=TRUE,SUBSTITUTE(C16,"&lt;","",1)*1,C16)&gt;VLOOKUP(A16,'SeuilsComparaison-EMT'!$C$5:$J$25,4,FALSE)=TRUE),(IF(ISTEXT(C16)=TRUE,SUBSTITUTE(C16,"&lt;","",1)*1,C16)-((IF(ISTEXT(C16)=TRUE,SUBSTITUTE(C16,"&lt;","",1)*1,C16)+IF(ISTEXT(E16)=TRUE,SUBSTITUTE(E16,"&lt;","",1)*1,E16))/2))/((IF(ISTEXT(C16)=TRUE,SUBSTITUTE(C16,"&lt;","",1)*1,C16)+IF(ISTEXT(E16)=TRUE,SUBSTITUTE(E16,"&lt;","",1),E16))/2),"-")))</f>
+        <v/>
       </c>
       <c r="H16" s="59"/>
       <c r="I16" s="39"/>
@@ -2924,8 +2952,8 @@
       <c r="E17" s="57"/>
       <c r="F17" s="58"/>
       <c r="G17" s="54" t="str">
-        <f t="shared" si="0"/>
-        <v>-</v>
+        <f>IF(OR(E17="",C17=""),"",IF(ISERROR(VLOOKUP(A17,'SeuilsComparaison-EMT'!$C$5:$J$25,4,FALSE)),"-",IF(OR(IF(ISTEXT(E17)=TRUE,SUBSTITUTE(E17,"&lt;","",1)*1,E17)&gt;VLOOKUP(A17,'SeuilsComparaison-EMT'!$C$5:$J$25,4,FALSE),IF(ISTEXT(C17)=TRUE,SUBSTITUTE(C17,"&lt;","",1)*1,C17)&gt;VLOOKUP(A17,'SeuilsComparaison-EMT'!$C$5:$J$25,4,FALSE)=TRUE),(IF(ISTEXT(C17)=TRUE,SUBSTITUTE(C17,"&lt;","",1)*1,C17)-((IF(ISTEXT(C17)=TRUE,SUBSTITUTE(C17,"&lt;","",1)*1,C17)+IF(ISTEXT(E17)=TRUE,SUBSTITUTE(E17,"&lt;","",1)*1,E17))/2))/((IF(ISTEXT(C17)=TRUE,SUBSTITUTE(C17,"&lt;","",1)*1,C17)+IF(ISTEXT(E17)=TRUE,SUBSTITUTE(E17,"&lt;","",1),E17))/2),"-")))</f>
+        <v/>
       </c>
       <c r="H17" s="59"/>
       <c r="I17" s="39"/>
@@ -2944,8 +2972,8 @@
       <c r="E18" s="57"/>
       <c r="F18" s="58"/>
       <c r="G18" s="54" t="str">
-        <f t="shared" si="0"/>
-        <v>-</v>
+        <f>IF(OR(E18="",C18=""),"",IF(ISERROR(VLOOKUP(A18,'SeuilsComparaison-EMT'!$C$5:$J$25,4,FALSE)),"-",IF(OR(IF(ISTEXT(E18)=TRUE,SUBSTITUTE(E18,"&lt;","",1)*1,E18)&gt;VLOOKUP(A18,'SeuilsComparaison-EMT'!$C$5:$J$25,4,FALSE),IF(ISTEXT(C18)=TRUE,SUBSTITUTE(C18,"&lt;","",1)*1,C18)&gt;VLOOKUP(A18,'SeuilsComparaison-EMT'!$C$5:$J$25,4,FALSE)=TRUE),(IF(ISTEXT(C18)=TRUE,SUBSTITUTE(C18,"&lt;","",1)*1,C18)-((IF(ISTEXT(C18)=TRUE,SUBSTITUTE(C18,"&lt;","",1)*1,C18)+IF(ISTEXT(E18)=TRUE,SUBSTITUTE(E18,"&lt;","",1)*1,E18))/2))/((IF(ISTEXT(C18)=TRUE,SUBSTITUTE(C18,"&lt;","",1)*1,C18)+IF(ISTEXT(E18)=TRUE,SUBSTITUTE(E18,"&lt;","",1),E18))/2),"-")))</f>
+        <v/>
       </c>
       <c r="H18" s="59"/>
       <c r="I18" s="39"/>
@@ -2964,8 +2992,8 @@
       <c r="E19" s="57"/>
       <c r="F19" s="58"/>
       <c r="G19" s="54" t="str">
-        <f t="shared" si="0"/>
-        <v>-</v>
+        <f>IF(OR(E19="",C19=""),"",IF(ISERROR(VLOOKUP(A19,'SeuilsComparaison-EMT'!$C$5:$J$25,4,FALSE)),"-",IF(OR(IF(ISTEXT(E19)=TRUE,SUBSTITUTE(E19,"&lt;","",1)*1,E19)&gt;VLOOKUP(A19,'SeuilsComparaison-EMT'!$C$5:$J$25,4,FALSE),IF(ISTEXT(C19)=TRUE,SUBSTITUTE(C19,"&lt;","",1)*1,C19)&gt;VLOOKUP(A19,'SeuilsComparaison-EMT'!$C$5:$J$25,4,FALSE)=TRUE),(IF(ISTEXT(C19)=TRUE,SUBSTITUTE(C19,"&lt;","",1)*1,C19)-((IF(ISTEXT(C19)=TRUE,SUBSTITUTE(C19,"&lt;","",1)*1,C19)+IF(ISTEXT(E19)=TRUE,SUBSTITUTE(E19,"&lt;","",1)*1,E19))/2))/((IF(ISTEXT(C19)=TRUE,SUBSTITUTE(C19,"&lt;","",1)*1,C19)+IF(ISTEXT(E19)=TRUE,SUBSTITUTE(E19,"&lt;","",1),E19))/2),"-")))</f>
+        <v/>
       </c>
       <c r="H19" s="59"/>
       <c r="I19" s="39"/>
@@ -2984,8 +3012,8 @@
       <c r="E20" s="57"/>
       <c r="F20" s="58"/>
       <c r="G20" s="54" t="str">
-        <f t="shared" si="0"/>
-        <v>-</v>
+        <f>IF(OR(E20="",C20=""),"",IF(ISERROR(VLOOKUP(A20,'SeuilsComparaison-EMT'!$C$5:$J$25,4,FALSE)),"-",IF(OR(IF(ISTEXT(E20)=TRUE,SUBSTITUTE(E20,"&lt;","",1)*1,E20)&gt;VLOOKUP(A20,'SeuilsComparaison-EMT'!$C$5:$J$25,4,FALSE),IF(ISTEXT(C20)=TRUE,SUBSTITUTE(C20,"&lt;","",1)*1,C20)&gt;VLOOKUP(A20,'SeuilsComparaison-EMT'!$C$5:$J$25,4,FALSE)=TRUE),(IF(ISTEXT(C20)=TRUE,SUBSTITUTE(C20,"&lt;","",1)*1,C20)-((IF(ISTEXT(C20)=TRUE,SUBSTITUTE(C20,"&lt;","",1)*1,C20)+IF(ISTEXT(E20)=TRUE,SUBSTITUTE(E20,"&lt;","",1)*1,E20))/2))/((IF(ISTEXT(C20)=TRUE,SUBSTITUTE(C20,"&lt;","",1)*1,C20)+IF(ISTEXT(E20)=TRUE,SUBSTITUTE(E20,"&lt;","",1),E20))/2),"-")))</f>
+        <v/>
       </c>
       <c r="H20" s="59"/>
       <c r="I20" s="39"/>
@@ -3004,8 +3032,8 @@
       <c r="E21" s="57"/>
       <c r="F21" s="58"/>
       <c r="G21" s="54" t="str">
-        <f t="shared" si="0"/>
-        <v>-</v>
+        <f>IF(OR(E21="",C21=""),"",IF(ISERROR(VLOOKUP(A21,'SeuilsComparaison-EMT'!$C$5:$J$25,4,FALSE)),"-",IF(OR(IF(ISTEXT(E21)=TRUE,SUBSTITUTE(E21,"&lt;","",1)*1,E21)&gt;VLOOKUP(A21,'SeuilsComparaison-EMT'!$C$5:$J$25,4,FALSE),IF(ISTEXT(C21)=TRUE,SUBSTITUTE(C21,"&lt;","",1)*1,C21)&gt;VLOOKUP(A21,'SeuilsComparaison-EMT'!$C$5:$J$25,4,FALSE)=TRUE),(IF(ISTEXT(C21)=TRUE,SUBSTITUTE(C21,"&lt;","",1)*1,C21)-((IF(ISTEXT(C21)=TRUE,SUBSTITUTE(C21,"&lt;","",1)*1,C21)+IF(ISTEXT(E21)=TRUE,SUBSTITUTE(E21,"&lt;","",1)*1,E21))/2))/((IF(ISTEXT(C21)=TRUE,SUBSTITUTE(C21,"&lt;","",1)*1,C21)+IF(ISTEXT(E21)=TRUE,SUBSTITUTE(E21,"&lt;","",1),E21))/2),"-")))</f>
+        <v/>
       </c>
       <c r="H21" s="59"/>
       <c r="I21" s="39"/>
@@ -3024,8 +3052,8 @@
       <c r="E22" s="57"/>
       <c r="F22" s="58"/>
       <c r="G22" s="54" t="str">
-        <f t="shared" si="0"/>
-        <v>-</v>
+        <f>IF(OR(E22="",C22=""),"",IF(ISERROR(VLOOKUP(A22,'SeuilsComparaison-EMT'!$C$5:$J$25,4,FALSE)),"-",IF(OR(IF(ISTEXT(E22)=TRUE,SUBSTITUTE(E22,"&lt;","",1)*1,E22)&gt;VLOOKUP(A22,'SeuilsComparaison-EMT'!$C$5:$J$25,4,FALSE),IF(ISTEXT(C22)=TRUE,SUBSTITUTE(C22,"&lt;","",1)*1,C22)&gt;VLOOKUP(A22,'SeuilsComparaison-EMT'!$C$5:$J$25,4,FALSE)=TRUE),(IF(ISTEXT(C22)=TRUE,SUBSTITUTE(C22,"&lt;","",1)*1,C22)-((IF(ISTEXT(C22)=TRUE,SUBSTITUTE(C22,"&lt;","",1)*1,C22)+IF(ISTEXT(E22)=TRUE,SUBSTITUTE(E22,"&lt;","",1)*1,E22))/2))/((IF(ISTEXT(C22)=TRUE,SUBSTITUTE(C22,"&lt;","",1)*1,C22)+IF(ISTEXT(E22)=TRUE,SUBSTITUTE(E22,"&lt;","",1),E22))/2),"-")))</f>
+        <v/>
       </c>
       <c r="H22" s="59"/>
       <c r="I22" s="39"/>
@@ -3044,8 +3072,8 @@
       <c r="E23" s="57"/>
       <c r="F23" s="58"/>
       <c r="G23" s="54" t="str">
-        <f t="shared" si="0"/>
-        <v>-</v>
+        <f>IF(OR(E23="",C23=""),"",IF(ISERROR(VLOOKUP(A23,'SeuilsComparaison-EMT'!$C$5:$J$25,4,FALSE)),"-",IF(OR(IF(ISTEXT(E23)=TRUE,SUBSTITUTE(E23,"&lt;","",1)*1,E23)&gt;VLOOKUP(A23,'SeuilsComparaison-EMT'!$C$5:$J$25,4,FALSE),IF(ISTEXT(C23)=TRUE,SUBSTITUTE(C23,"&lt;","",1)*1,C23)&gt;VLOOKUP(A23,'SeuilsComparaison-EMT'!$C$5:$J$25,4,FALSE)=TRUE),(IF(ISTEXT(C23)=TRUE,SUBSTITUTE(C23,"&lt;","",1)*1,C23)-((IF(ISTEXT(C23)=TRUE,SUBSTITUTE(C23,"&lt;","",1)*1,C23)+IF(ISTEXT(E23)=TRUE,SUBSTITUTE(E23,"&lt;","",1)*1,E23))/2))/((IF(ISTEXT(C23)=TRUE,SUBSTITUTE(C23,"&lt;","",1)*1,C23)+IF(ISTEXT(E23)=TRUE,SUBSTITUTE(E23,"&lt;","",1),E23))/2),"-")))</f>
+        <v/>
       </c>
       <c r="H23" s="59"/>
       <c r="I23" s="39"/>
@@ -3064,8 +3092,8 @@
       <c r="E24" s="57"/>
       <c r="F24" s="58"/>
       <c r="G24" s="54" t="str">
-        <f t="shared" si="0"/>
-        <v>-</v>
+        <f>IF(OR(E24="",C24=""),"",IF(ISERROR(VLOOKUP(A24,'SeuilsComparaison-EMT'!$C$5:$J$25,4,FALSE)),"-",IF(OR(IF(ISTEXT(E24)=TRUE,SUBSTITUTE(E24,"&lt;","",1)*1,E24)&gt;VLOOKUP(A24,'SeuilsComparaison-EMT'!$C$5:$J$25,4,FALSE),IF(ISTEXT(C24)=TRUE,SUBSTITUTE(C24,"&lt;","",1)*1,C24)&gt;VLOOKUP(A24,'SeuilsComparaison-EMT'!$C$5:$J$25,4,FALSE)=TRUE),(IF(ISTEXT(C24)=TRUE,SUBSTITUTE(C24,"&lt;","",1)*1,C24)-((IF(ISTEXT(C24)=TRUE,SUBSTITUTE(C24,"&lt;","",1)*1,C24)+IF(ISTEXT(E24)=TRUE,SUBSTITUTE(E24,"&lt;","",1)*1,E24))/2))/((IF(ISTEXT(C24)=TRUE,SUBSTITUTE(C24,"&lt;","",1)*1,C24)+IF(ISTEXT(E24)=TRUE,SUBSTITUTE(E24,"&lt;","",1),E24))/2),"-")))</f>
+        <v/>
       </c>
       <c r="H24" s="59"/>
       <c r="I24" s="39"/>
@@ -3084,8 +3112,8 @@
       <c r="E25" s="57"/>
       <c r="F25" s="58"/>
       <c r="G25" s="54" t="str">
-        <f t="shared" si="0"/>
-        <v>-</v>
+        <f>IF(OR(E25="",C25=""),"",IF(ISERROR(VLOOKUP(A25,'SeuilsComparaison-EMT'!$C$5:$J$25,4,FALSE)),"-",IF(OR(IF(ISTEXT(E25)=TRUE,SUBSTITUTE(E25,"&lt;","",1)*1,E25)&gt;VLOOKUP(A25,'SeuilsComparaison-EMT'!$C$5:$J$25,4,FALSE),IF(ISTEXT(C25)=TRUE,SUBSTITUTE(C25,"&lt;","",1)*1,C25)&gt;VLOOKUP(A25,'SeuilsComparaison-EMT'!$C$5:$J$25,4,FALSE)=TRUE),(IF(ISTEXT(C25)=TRUE,SUBSTITUTE(C25,"&lt;","",1)*1,C25)-((IF(ISTEXT(C25)=TRUE,SUBSTITUTE(C25,"&lt;","",1)*1,C25)+IF(ISTEXT(E25)=TRUE,SUBSTITUTE(E25,"&lt;","",1)*1,E25))/2))/((IF(ISTEXT(C25)=TRUE,SUBSTITUTE(C25,"&lt;","",1)*1,C25)+IF(ISTEXT(E25)=TRUE,SUBSTITUTE(E25,"&lt;","",1),E25))/2),"-")))</f>
+        <v/>
       </c>
       <c r="H25" s="59"/>
       <c r="I25" s="39"/>
@@ -3104,8 +3132,8 @@
       <c r="E26" s="66"/>
       <c r="F26" s="67"/>
       <c r="G26" s="54" t="str">
-        <f t="shared" si="0"/>
-        <v>-</v>
+        <f>IF(OR(E26="",C26=""),"",IF(ISERROR(VLOOKUP(A26,'SeuilsComparaison-EMT'!$C$5:$J$25,4,FALSE)),"-",IF(OR(IF(ISTEXT(E26)=TRUE,SUBSTITUTE(E26,"&lt;","",1)*1,E26)&gt;VLOOKUP(A26,'SeuilsComparaison-EMT'!$C$5:$J$25,4,FALSE),IF(ISTEXT(C26)=TRUE,SUBSTITUTE(C26,"&lt;","",1)*1,C26)&gt;VLOOKUP(A26,'SeuilsComparaison-EMT'!$C$5:$J$25,4,FALSE)=TRUE),(IF(ISTEXT(C26)=TRUE,SUBSTITUTE(C26,"&lt;","",1)*1,C26)-((IF(ISTEXT(C26)=TRUE,SUBSTITUTE(C26,"&lt;","",1)*1,C26)+IF(ISTEXT(E26)=TRUE,SUBSTITUTE(E26,"&lt;","",1)*1,E26))/2))/((IF(ISTEXT(C26)=TRUE,SUBSTITUTE(C26,"&lt;","",1)*1,C26)+IF(ISTEXT(E26)=TRUE,SUBSTITUTE(E26,"&lt;","",1),E26))/2),"-")))</f>
+        <v/>
       </c>
       <c r="H26" s="59"/>
       <c r="I26" s="39"/>
@@ -3124,8 +3152,8 @@
       <c r="E27" s="66"/>
       <c r="F27" s="67"/>
       <c r="G27" s="54" t="str">
-        <f t="shared" si="0"/>
-        <v>-</v>
+        <f>IF(OR(E27="",C27=""),"",IF(ISERROR(VLOOKUP(A27,'SeuilsComparaison-EMT'!$C$5:$J$25,4,FALSE)),"-",IF(OR(IF(ISTEXT(E27)=TRUE,SUBSTITUTE(E27,"&lt;","",1)*1,E27)&gt;VLOOKUP(A27,'SeuilsComparaison-EMT'!$C$5:$J$25,4,FALSE),IF(ISTEXT(C27)=TRUE,SUBSTITUTE(C27,"&lt;","",1)*1,C27)&gt;VLOOKUP(A27,'SeuilsComparaison-EMT'!$C$5:$J$25,4,FALSE)=TRUE),(IF(ISTEXT(C27)=TRUE,SUBSTITUTE(C27,"&lt;","",1)*1,C27)-((IF(ISTEXT(C27)=TRUE,SUBSTITUTE(C27,"&lt;","",1)*1,C27)+IF(ISTEXT(E27)=TRUE,SUBSTITUTE(E27,"&lt;","",1)*1,E27))/2))/((IF(ISTEXT(C27)=TRUE,SUBSTITUTE(C27,"&lt;","",1)*1,C27)+IF(ISTEXT(E27)=TRUE,SUBSTITUTE(E27,"&lt;","",1),E27))/2),"-")))</f>
+        <v/>
       </c>
       <c r="H27" s="59"/>
       <c r="I27" s="39"/>
@@ -3144,8 +3172,8 @@
       <c r="E28" s="66"/>
       <c r="F28" s="67"/>
       <c r="G28" s="54" t="str">
-        <f t="shared" si="0"/>
-        <v>-</v>
+        <f>IF(OR(E28="",C28=""),"",IF(ISERROR(VLOOKUP(A28,'SeuilsComparaison-EMT'!$C$5:$J$25,4,FALSE)),"-",IF(OR(IF(ISTEXT(E28)=TRUE,SUBSTITUTE(E28,"&lt;","",1)*1,E28)&gt;VLOOKUP(A28,'SeuilsComparaison-EMT'!$C$5:$J$25,4,FALSE),IF(ISTEXT(C28)=TRUE,SUBSTITUTE(C28,"&lt;","",1)*1,C28)&gt;VLOOKUP(A28,'SeuilsComparaison-EMT'!$C$5:$J$25,4,FALSE)=TRUE),(IF(ISTEXT(C28)=TRUE,SUBSTITUTE(C28,"&lt;","",1)*1,C28)-((IF(ISTEXT(C28)=TRUE,SUBSTITUTE(C28,"&lt;","",1)*1,C28)+IF(ISTEXT(E28)=TRUE,SUBSTITUTE(E28,"&lt;","",1)*1,E28))/2))/((IF(ISTEXT(C28)=TRUE,SUBSTITUTE(C28,"&lt;","",1)*1,C28)+IF(ISTEXT(E28)=TRUE,SUBSTITUTE(E28,"&lt;","",1),E28))/2),"-")))</f>
+        <v/>
       </c>
       <c r="H28" s="59"/>
       <c r="I28" s="39"/>
@@ -3164,8 +3192,8 @@
       <c r="E29" s="66"/>
       <c r="F29" s="67"/>
       <c r="G29" s="54" t="str">
-        <f t="shared" si="0"/>
-        <v>-</v>
+        <f>IF(OR(E29="",C29=""),"",IF(ISERROR(VLOOKUP(A29,'SeuilsComparaison-EMT'!$C$5:$J$25,4,FALSE)),"-",IF(OR(IF(ISTEXT(E29)=TRUE,SUBSTITUTE(E29,"&lt;","",1)*1,E29)&gt;VLOOKUP(A29,'SeuilsComparaison-EMT'!$C$5:$J$25,4,FALSE),IF(ISTEXT(C29)=TRUE,SUBSTITUTE(C29,"&lt;","",1)*1,C29)&gt;VLOOKUP(A29,'SeuilsComparaison-EMT'!$C$5:$J$25,4,FALSE)=TRUE),(IF(ISTEXT(C29)=TRUE,SUBSTITUTE(C29,"&lt;","",1)*1,C29)-((IF(ISTEXT(C29)=TRUE,SUBSTITUTE(C29,"&lt;","",1)*1,C29)+IF(ISTEXT(E29)=TRUE,SUBSTITUTE(E29,"&lt;","",1)*1,E29))/2))/((IF(ISTEXT(C29)=TRUE,SUBSTITUTE(C29,"&lt;","",1)*1,C29)+IF(ISTEXT(E29)=TRUE,SUBSTITUTE(E29,"&lt;","",1),E29))/2),"-")))</f>
+        <v/>
       </c>
       <c r="H29" s="59"/>
       <c r="I29" s="39"/>
@@ -3183,7 +3211,10 @@
       <c r="D30" s="65"/>
       <c r="E30" s="66"/>
       <c r="F30" s="67"/>
-      <c r="G30" s="54"/>
+      <c r="G30" s="54" t="str">
+        <f>IF(OR(E30="",C30=""),"",IF(ISERROR(VLOOKUP(A30,'SeuilsComparaison-EMT'!$C$5:$J$25,4,FALSE)),"-",IF(OR(IF(ISTEXT(E30)=TRUE,SUBSTITUTE(E30,"&lt;","",1)*1,E30)&gt;VLOOKUP(A30,'SeuilsComparaison-EMT'!$C$5:$J$25,4,FALSE),IF(ISTEXT(C30)=TRUE,SUBSTITUTE(C30,"&lt;","",1)*1,C30)&gt;VLOOKUP(A30,'SeuilsComparaison-EMT'!$C$5:$J$25,4,FALSE)=TRUE),(IF(ISTEXT(C30)=TRUE,SUBSTITUTE(C30,"&lt;","",1)*1,C30)-((IF(ISTEXT(C30)=TRUE,SUBSTITUTE(C30,"&lt;","",1)*1,C30)+IF(ISTEXT(E30)=TRUE,SUBSTITUTE(E30,"&lt;","",1)*1,E30))/2))/((IF(ISTEXT(C30)=TRUE,SUBSTITUTE(C30,"&lt;","",1)*1,C30)+IF(ISTEXT(E30)=TRUE,SUBSTITUTE(E30,"&lt;","",1),E30))/2),"-")))</f>
+        <v/>
+      </c>
       <c r="H30" s="59"/>
       <c r="I30" s="39"/>
       <c r="J30" s="40"/>
@@ -3200,28 +3231,31 @@
       <c r="D31" s="65"/>
       <c r="E31" s="66"/>
       <c r="F31" s="67"/>
-      <c r="G31" s="54"/>
+      <c r="G31" s="54" t="str">
+        <f>IF(OR(E31="",C31=""),"",IF(ISERROR(VLOOKUP(A31,'SeuilsComparaison-EMT'!$C$5:$J$25,4,FALSE)),"-",IF(OR(IF(ISTEXT(E31)=TRUE,SUBSTITUTE(E31,"&lt;","",1)*1,E31)&gt;VLOOKUP(A31,'SeuilsComparaison-EMT'!$C$5:$J$25,4,FALSE),IF(ISTEXT(C31)=TRUE,SUBSTITUTE(C31,"&lt;","",1)*1,C31)&gt;VLOOKUP(A31,'SeuilsComparaison-EMT'!$C$5:$J$25,4,FALSE)=TRUE),(IF(ISTEXT(C31)=TRUE,SUBSTITUTE(C31,"&lt;","",1)*1,C31)-((IF(ISTEXT(C31)=TRUE,SUBSTITUTE(C31,"&lt;","",1)*1,C31)+IF(ISTEXT(E31)=TRUE,SUBSTITUTE(E31,"&lt;","",1)*1,E31))/2))/((IF(ISTEXT(C31)=TRUE,SUBSTITUTE(C31,"&lt;","",1)*1,C31)+IF(ISTEXT(E31)=TRUE,SUBSTITUTE(E31,"&lt;","",1),E31))/2),"-")))</f>
+        <v/>
+      </c>
       <c r="H31" s="59"/>
       <c r="I31" s="39"/>
       <c r="J31" s="40"/>
     </row>
     <row r="32" spans="1:10" ht="14.7" thickBot="1" x14ac:dyDescent="0.55000000000000004">
-      <c r="A32" s="68" t="s">
+      <c r="A32" s="98" t="s">
         <v>37</v>
       </c>
-      <c r="B32" s="49">
+      <c r="B32" s="99">
         <f>VLOOKUP(A32, 'SeuilsComparaison-EMT'!$C$5:$E$28, 3, FALSE)</f>
         <v>5</v>
       </c>
-      <c r="C32" s="69"/>
-      <c r="D32" s="70"/>
-      <c r="E32" s="71"/>
-      <c r="F32" s="72"/>
-      <c r="G32" s="73" t="str">
-        <f t="shared" ref="G32" si="1" xml:space="preserve"> IF(E32&gt;0,(C32-E32)/E32,"-")</f>
-        <v>-</v>
-      </c>
-      <c r="H32" s="74"/>
+      <c r="C32" s="68"/>
+      <c r="D32" s="69"/>
+      <c r="E32" s="70"/>
+      <c r="F32" s="71"/>
+      <c r="G32" s="100" t="str">
+        <f>IF(OR(E32="",C32=""),"",IF(ISERROR(VLOOKUP(A32,'SeuilsComparaison-EMT'!$C$5:$J$25,4,FALSE)),"-",IF(OR(IF(ISTEXT(E32)=TRUE,SUBSTITUTE(E32,"&lt;","",1)*1,E32)&gt;VLOOKUP(A32,'SeuilsComparaison-EMT'!$C$5:$J$25,4,FALSE),IF(ISTEXT(C32)=TRUE,SUBSTITUTE(C32,"&lt;","",1)*1,C32)&gt;VLOOKUP(A32,'SeuilsComparaison-EMT'!$C$5:$J$25,4,FALSE)=TRUE),(IF(ISTEXT(C32)=TRUE,SUBSTITUTE(C32,"&lt;","",1)*1,C32)-((IF(ISTEXT(C32)=TRUE,SUBSTITUTE(C32,"&lt;","",1)*1,C32)+IF(ISTEXT(E32)=TRUE,SUBSTITUTE(E32,"&lt;","",1)*1,E32))/2))/((IF(ISTEXT(C32)=TRUE,SUBSTITUTE(C32,"&lt;","",1)*1,C32)+IF(ISTEXT(E32)=TRUE,SUBSTITUTE(E32,"&lt;","",1),E32))/2),"-")))</f>
+        <v/>
+      </c>
+      <c r="H32" s="72"/>
       <c r="I32" s="39"/>
       <c r="J32" s="40"/>
     </row>
@@ -3252,26 +3286,26 @@
       <c r="J34" s="40"/>
     </row>
     <row r="35" spans="1:10" x14ac:dyDescent="0.5">
-      <c r="A35" s="84"/>
-      <c r="B35" s="84"/>
-      <c r="C35" s="84"/>
-      <c r="D35" s="84"/>
-      <c r="E35" s="84"/>
-      <c r="F35" s="84"/>
-      <c r="G35" s="84"/>
-      <c r="H35" s="84"/>
+      <c r="A35" s="80"/>
+      <c r="B35" s="80"/>
+      <c r="C35" s="80"/>
+      <c r="D35" s="80"/>
+      <c r="E35" s="80"/>
+      <c r="F35" s="80"/>
+      <c r="G35" s="80"/>
+      <c r="H35" s="80"/>
       <c r="I35" s="39"/>
       <c r="J35" s="40"/>
     </row>
     <row r="36" spans="1:10" x14ac:dyDescent="0.5">
-      <c r="A36" s="84"/>
-      <c r="B36" s="84"/>
-      <c r="C36" s="84"/>
-      <c r="D36" s="84"/>
-      <c r="E36" s="84"/>
-      <c r="F36" s="84"/>
-      <c r="G36" s="84"/>
-      <c r="H36" s="84"/>
+      <c r="A36" s="80"/>
+      <c r="B36" s="80"/>
+      <c r="C36" s="80"/>
+      <c r="D36" s="80"/>
+      <c r="E36" s="80"/>
+      <c r="F36" s="80"/>
+      <c r="G36" s="80"/>
+      <c r="H36" s="80"/>
       <c r="I36" s="39"/>
       <c r="J36" s="40"/>
     </row>
@@ -3289,6 +3323,13 @@
     </row>
   </sheetData>
   <mergeCells count="18">
+    <mergeCell ref="C2:D2"/>
+    <mergeCell ref="E2:F2"/>
+    <mergeCell ref="G2:H2"/>
+    <mergeCell ref="A3:B3"/>
+    <mergeCell ref="C3:D3"/>
+    <mergeCell ref="E3:F3"/>
+    <mergeCell ref="A2:B2"/>
     <mergeCell ref="A35:H36"/>
     <mergeCell ref="G4:H4"/>
     <mergeCell ref="G5:H5"/>
@@ -3300,13 +3341,6 @@
     <mergeCell ref="F7:F10"/>
     <mergeCell ref="G9:G10"/>
     <mergeCell ref="H9:H10"/>
-    <mergeCell ref="C2:D2"/>
-    <mergeCell ref="E2:F2"/>
-    <mergeCell ref="G2:H2"/>
-    <mergeCell ref="A3:B3"/>
-    <mergeCell ref="C3:D3"/>
-    <mergeCell ref="E3:F3"/>
-    <mergeCell ref="A2:B2"/>
   </mergeCells>
   <conditionalFormatting sqref="F11:F32">
     <cfRule type="cellIs" dxfId="2" priority="3" operator="equal">

</xml_diff>